<commit_message>
Updated README as a document for this project
</commit_message>
<xml_diff>
--- a/Rory Testing Sheet 2024.xlsx
+++ b/Rory Testing Sheet 2024.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B202"/>
+  <dimension ref="A1:B216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2867,6 +2867,174 @@
         </is>
       </c>
     </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>https://markets.businessinsider.com/news/stocks/go-investor-alert-bronstein-gewirtz-and-grossman-llc-announces-that-grocery-outlet-holding-corp-investors-have-opportunity-to-lead-class-action-lawsuit-1034362052</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>GO INVESTOR ALERT: Bronstein, Gewirtz and Grossman, LLC Announces that Grocery Outlet Holding Corp. Investors Have Opportunity to Lead Class Action Lawsuit!</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>https://www.wdtn.com/top-stories/county-sues-daytons-water-department-for-alleged-breach-of-contact/</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>County sues Dayton’s Water Department for alleged ‘breach of contract’</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>https://www.whio.com/news/local/county-sues-city-water-department-breach-contract/HHKYSGJYDND2VNY66QRNECHTSY/</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Montgomery County sues City of Dayton Water Department for breach of contract</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>https://dailyfly.com/republicans-target-100-billion-in-alleged-covid-era-unemployment-fraud/</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Republicans Target $100 Billion in Alleged COVID-Era Unemployment Fraud</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>https://www.kcentv.com/article/news/crime/tarver-elementary-teacher-placed-leave-allegations-misconduct/500-b480a191-9ade-4970-b0de-1f5d4d9cd3fb</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Tarver Elementary teacher placed on leave after allegations of misconduct</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>https://www.theglobeandmail.com/canada/alberta/article-alberta-cabinet-minister-calls-for-removal-of-health-minister-amid/</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Alberta cabinet minister calls for removal of health minister amid corruption scandal</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>https://www.postcourier.com.pg/ceo-charged-by-ncd-police/</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>CEO charged by NCD Police</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>https://news.sd.gov/news?id=news_kb_article_view&amp;sys_id=9e0a23101bbf5e90f6142062f54bcb53</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>AG Jackley States Lawsuit Will Not Eliminate Section 504 School Disability Accommodations</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>https://www.wsmv.com/2025/02/14/wayne-county-deputy-awarded-17m-lawsuit-against-driver-who-hit-hit-while-directing-traffic/</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Wayne County deputy awarded $1.7M in lawsuit against driver who hit hit while directing traffic</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>https://www.wlns.com/news/michigan-joins-lawsuit-to-block-transgender-military-ban/</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Michigan Attorney General files brief in support of lawsuit to block transgender military ban</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>https://lawnews.hofstra.edu/2025/02/14/prof-irina-manta-discusses-lawsuit-against-ai-company-for-alleged-copyright-infringement/</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Prof. Irina Manta Discusses Lawsuit Against AI Company for Alleged Copyright Infringement</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>https://www.bbc.com/news/articles/cn93rnnjw4zo</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Seventh attorney resigns after refusing to dismiss case against NYC Mayor Eric Adams</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>https://www.bbc.com/news/articles/cnvqlgyq7qvo</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Farsley Celtic chairman resigns after abuse from supporters</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>https://www.thewetumpkaherald.com/news/local-lawyer-arrested-for-harassment/article_e2147ad8-eb1f-11ef-b37b-a776e2f708f0.html</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Local lawyer arrested for harassment</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the Connection error from the exist of driver
</commit_message>
<xml_diff>
--- a/Rory Testing Sheet 2024.xlsx
+++ b/Rory Testing Sheet 2024.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B227"/>
+  <dimension ref="A1:B246"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3167,6 +3167,234 @@
         </is>
       </c>
     </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>https://www.dakotanewsnow.com/2025/02/14/jackley-clarifies-focus-multi-state-section-504-lawsuit/</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Jackley clarifies the focus of multi-state Section 504 lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>https://www.dallasnews.com/news/2025/02/14/lawsuit-filed-friday-against-keller-isd-alleges-violations-of-voting-rights-act/</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Lawsuit filed against Keller ISD alleges violations of Voting Rights Act</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>https://arkansasadvocate.com/briefs/20-red-states-including-arkansas-back-doge-in-lawsuit-challenging-access-to-treasury-system/</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>20 red states, including Arkansas, back DOGE in lawsuit challenging access to Treasury system</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>https://lawnews.hofstra.edu/2025/02/14/prof-james-sample-explains-federal-lawsuit-against-new-yorks-green-light-law/</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Prof. James Sample Explains Federal Lawsuit Against New York’s Green Light Law</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>https://thedaily.case.edu/laws-sharona-hoffman-discusses-an-insulin-lawsuit-recently-filed-by-the-city-of-columbus/</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Law’s Sharona Hoffman discusses an insulin lawsuit recently filed by the City of Columbus</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>https://www.alexcityoutlook.com/elmore-county-lawyer-arrested-for-harassment/article_87d9737c-4b06-5dae-aa75-326147315dd6.html</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Elmore County lawyer arrested for harassment</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>https://www.yahoo.com/entertainment/fla-lawyer-allegedly-smashed-plate-141907407.html</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Fla. Lawyer Allegedly Smashed Plate Over Fellow Wedding Attendee’s Head When He Allowed Others to Cut in Buffet Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>https://www.whas11.com/video/news/local/indiana/attorney-general-threatening-legal-action-against-indianapolis-authorities-schools/417-bcc673c1-09e4-4abc-b8fc-738431a1ec29</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Attorney general threatening legal action against Indianapolis authorities, schools</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>https://edmontonjournal.com/news/politics/outrageous-and-false-how-those-named-in-the-ahs-lawsuit-are-responding-to-the-allegations</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>'Outrageous and false': How those named in the AHS lawsuit are responding to the allegations</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>https://www.billboard.com/music/rb-hip-hop/glorilla-bbl-glorious-tour-1235903399/</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>GloRilla Denies BBL Rumors as She Preps for ‘The Glorious Tour’</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>https://theprint.in/india/ed-seizes-rs-170-cr-worth-bank-deposits-in-probe-against-fraud-forex-trading-platform/2492261/</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>ED seizes Rs 170-cr worth bank deposits in probe against ‘fraud’ forex trading platform</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>https://www.notus.org/whitehouse/doge-posts-then-redacts-sensitive-hud-contract-data</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>DOGE Posts — Then Redacts — What Appears to Be Sensitive HUD Contract Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>https://www.fox44news.com/news/local-news/bell-county/tarver-elementary-teacher-placed-on-leave-amid-misconduct-allegations/</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Tarver Elementary teacher placed on leave amid misconduct allegations - KWKT</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>https://mynbc15.com/news/local/mobile-mardi-gras-queen-accused-of-nearly-15m-embezzlement-scheme</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Mobile Mardi Gras queen accused of nearly $1.5M embezzlement scheme</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>https://www.texomashomepage.com/news/crime/vernon-business-owner-accused-of-child-sex-crimes/</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Vernon business owner accused of child sex crimes - KFDX</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>https://www.msn.com/en-us/news/crime/mass-daycare-co-owner-accused-of-assaulting-children-in-her-care/ar-AA1yyDPu</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Mass. daycare co-owner accused of assaulting children in her care</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>https://www.m9.news/usa-news/b1-b2-visa-revoked-traveler-finds-out-at-airport/</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>B1/B2 Visa Revoked -Traveler Finds Out at Airport</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>https://www.bbc.com/news/articles/c9qj8gelgz8o</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>EHarley Street: Calls for inquiry into GP management 'scandal'</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>https://www.newsx.com/entertainment/netflix-addresses-controversy-surrounding-karla-sofia-gascon-amid-emilia-perez-scandal/</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Netflix Addresses Controversy Surrounding Karla Sofía Gascón Amid ‘Emilia Pérez’ Scandal</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added a function to remove duplicated articles before append to Rory file and what includes negative words
</commit_message>
<xml_diff>
--- a/Rory Testing Sheet 2024.xlsx
+++ b/Rory Testing Sheet 2024.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B323"/>
+  <dimension ref="A1:B491"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,7 +440,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="340" customWidth="1" min="1" max="1"/>
-    <col width="180" customWidth="1" min="2" max="2"/>
+    <col width="214" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4319,6 +4319,2022 @@
         </is>
       </c>
     </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>https://thenationaldesk.com/top-videos/expert-blasts-fla-teacher-for-response-after-backlash-for-showing-disney-movie-to-class-gay-character-in-film-strange-world-jenna-barbee-parents-give-up-rights-when-they-send-their-kids-to-public-schools-investigation-education?jw_start={seek_to_second_number}</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Expert blasts Fla. teacher for response after backlash for showing Disney movie to class</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>https://www.dailymail.co.uk/news/article-14400637/BT-thousands-customers-report-internet-outages-unable-access-emails.html</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>BT is DOWN: Company issues statement as thousands of customers report internet outages and being unable to acc</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>https://www.gamereactor.eu/armie-hammer-speaks-up-and-rejects-cannibal-allegations-1495503/</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Armie Hammer speaks up and rejects cannibal allegations</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>https://www.hpbl.co.in/news/ripple-xrp-price-faces-turmoil-will-legal-clarity-spark-a-rebound/</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Ripple (XRP) Price Faces Turmoil: Will Legal Clarity Spark a Rebound? – Coin Trading</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>https://www.communitynewspapergroup.com/news/nation/france-pm-vows-to-help-probe-boarding-school-paedophilia-allegations/article_9fcc6db9-f216-5b6d-8a10-14178a711aa7.html</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>France PM vows to help probe boarding school paedophilia allegations</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>https://www.yahoo.com/news/tarver-elementary-teacher-placed-leave-225803697.html</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Tarver Elementary teacher placed on leave amid misconduct allegations</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>https://www.thenews.com.pk/latest/1283204-justin-baldoni-seeks-escape-as-blake-lively-legal-drama-heats-up</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Justin Baldoni seeks escape as Blake Lively legal drama heats up</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>https://www.yahoo.com/news/doj-files-motion-dismiss-charges-122814701.html</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>DOJ files motion to dismiss charges against NYC mayor</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>https://nypost.com/2025/02/15/us-news/doge-wins-access-to-sensitive-labor-hhs-and-cfpb-data-from-federal-judge/</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>DOGE wins access to sensitive Labor Department, HHS and CFPB data from federal judge</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>https://www.businesswire.com/news/home/20250215649914/en/APLT-Deadline-Rosen-Law-Firm-Urges-Applied-Therapeutics-Inc.-NASDAQ-APLT-Investors-to-Contact-the-Firm-for-Information-About-Their-Rights</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>APLT Deadline: Rosen Law Firm Urges Applied Therapeutics, Inc. (NASDAQ: APLT) Investors to Contact the Firm for Information About Their Rights</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>https://www.globenewswire.com/news-release/2025/02/15/3026933/0/en/TMDX-INVESTOR-ALERT-Robbins-Geller-Rudman-Dowd-LLP-Announces-that-TransMedics-Group-Inc-Investors-with-Substantial-Losses-Have-Opportunity-to-Lead-the-TransMedics-Class-Action-Laws.html</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>TMDX INVESTOR ALERT: Robbins Geller Rudman &amp; Dowd LLP</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>https://www.hrmorning.com/news/new-lawsuit-starbucks-dei-policy/</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>New Lawsuit Challenges Starbucks’ DEI Policy – 5 Keys to Watch</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>https://timesofindia.indiatimes.com/city/chandigarh/immigration-firm-owner-arrested-for-fraud/articleshow/118285270.cms</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Immigration firm owner arrested for fraud</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>https://evrimagaci.org/tpg/infosys-faces-backlash-after-mass-layoffs-of-trainees-197877</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Infosys Faces Backlash After Mass Layoffs Of Trainees</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>https://www.aol.com/over-1-4-million-embezzled-171636956.html</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Over $1.4 million embezzled from Hardware Sales in Bellingham</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>https://www.dailymail.co.uk/news/article-14400637/BT-thousands-customers-report-internet-outages-unable-access-emails.html</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>BT is DOWN: thousands of customers report internet outages</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>https://www.news24.com/news24/southafrica/news/principal-of-top-pretoria-school-to-face-six-charges-of-misconduct-at-disciplinary-hearing-20250215</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Principal of top Pretoria school to face six charges of misconduct at disciplinary hearing</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>https://www.mykxlg.com/news/state/lawsuit-on-gender-dysphoria-classification-wont-affect-student-disability-services-in-south-dakota/article_2f00db98-ebcf-11ef-903e-bf8f061ebf51.html</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Lawsuit on Gender Dysphoria Classification Won't Affect Student Disability Services in South Dakota</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>https://www.blackenterprise.com/sexual-assault-lawsuit-against-jay-z-diddy-dismissed-by-jane-doe/</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Sexual Assault Lawsuit Against Jay-Z And Diddy Dropped By Jane Doe</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>https://www.msn.com/en-us/news/us/religious-organizations-including-jews-catholics-mennonites-file-lawsuit-to-prevent-immigration-raids-in-houses-of-worship/ar-AA1yQuUn?ocid=iehp</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Religious Organizations Including Jews, Catholics, Mennonites, File Lawsuit To Prevent Immigration Raids In Houses Of Worship</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>https://www.morningstar.com/news/pr-newswire/20250213ny18142/march-31-2025-deadline-contact-the-gross-law-firm-to-join-class-action-suit-against-go</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>March 31, 2025 Deadline: Contact The Gross Law Firm to Join Class Action Suit Against GO</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>https://ironcountytoday.com/2025/02/15/cedar-city-man-arrested-following-multiple-allegations-of-sexual-assault/</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Cedar City Man Arrested Following Multiple Allegations of Sexual Assault</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>https://www.newser.com/story/364332/man-charged-in-ceos-death-posts-thanks-on-new-website.html</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Man Charged in CEO's Death Posts Thanks on New Website</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>https://abcnews.go.com/Politics/video/doj-files-motion-dismiss-charges-nyc-mayor-118860869</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Video DOJ files motion to dismiss charges against NYC mayor</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>http://www.msn.com/en-us/news/politics/ford-13-other-state-ags-file-suit-to-strip-musk-of-executive-access/ar-AA1z0ttK?apiversion=v2&amp;noservercache=1&amp;domshim=1&amp;renderwebcomponents=1&amp;wcseo=1&amp;batchservertelemetry=1&amp;noservertelemetry=1</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Ford, 13 other state AGs, file suit to strip Musk of executive access</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/novelist-musician-and-pioneer-hits-new-milestone--80-year-old-rick-bleiweiss-says-dream-bigger-302377562.html</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>NOVELIST, MUSICIAN AND PIONEER HITS NEW MILESTONE - 80-YEAR-OLD RICK BLEIWEISS SAYS "DREAM BIGGER"</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>https://www.cryptoninjas.net/news/pantera-founder-faces-850m-tax-investigation-puerto-rico-tax-haven-in-the-crosshairs/</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Pantera Founder Faces $850M Tax Investigation: Puerto Rico Tax Haven in the Crosshairs</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>https://www.hotnewhiphop.com/885829-jay-z-lawyer-statement-sexual-assault-lawsuit-dropped-hip-hop-news</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Jay-Z's Lawyer Issues Statement After Tony Buzbee Drops Hov's Sexual Assault Lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>https://taskandpurpose.com/military-life/coast-guard-data-breach-pay/</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Coast Guard hit with data breach, impacting pay for more than 1,100 members</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>https://fox2now.com/news/missouri/deputy-accused-of-misconduct-with-inmate-at-st-louis-justice-center/</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Deputy accused of misconduct with inmate at St. Louis Justice Center</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>https://www.housingwire.com/articles/judge-blocks-cfpb-firings-amid-treasury-labor-union-lawsuit/</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Judge blocks CFPB firings amid Treasury labor union lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>https://www.washingtonpost.com/business/2025/02/15/cfpb-layoffs-halted/</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Layoffs halted at CFPB for now as judge considers union’s lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/fmc-purchasers-have-opportunity-to-lead-fmc-corporation-securities-fraud-lawsuit-302377223.html</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>FMC Purchasers Have Opportunity to Lead FMC Corporation Securities Fraud Lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>https://www.irishnews.com/sport/soccer/burtons-udoka-godwin-malife-suffers-alleged-racist-abuse-at-bristol-rovers-5G4APN5BUJKONIT4YXZSYE3CYM/</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Burton’s Udoka Godwin-Malife suffers alleged racist abuse at Bristol Rovers</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>https://www.france24.com/en/video/20250215-fran%C3%A7ois-bayrou-battles-to-contain-scandal</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>François Bayrou battles to contain scandal</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>https://www.globenewswire.com/news-release/2025/02/14/3026771/0/en/investor-alert-class-action-lawsuit-filed-on-behalf-of-fmc-corporation-fmc-investors-holzer-holzer-llc-encourages-investors-with-significant-losses-to-contact-the-firm.html</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>INVESTOR ALERT: Class Action Lawsuit Filed on Behalf of FMC</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>https://www.lemonde.fr/en/france/article/2025/02/15/french-pm-vows-to-help-probe-boarding-school-abuse-allegations-repeats-he-was-not-aware_6738201_7.html</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>French PM vows to help probe boarding school abuse allegations, repeats he was 'not aware'</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>https://www.breakingbelizenews.com/2025/02/15/ivan-ayuso-sentenced-to-five-years-for-embezzling-over-1m-from-gob/</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Ivan Ayuso sentenced to five years for embezzling over $1M from GOB</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>https://timesofindia.indiatimes.com/city/hyderabad/ed-facilitates-restitution-of-31-cr-properties-to-sbi-in-pmla-case/articleshow/118284249.cms</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>ED facilitates restitution of 31 cr properties to SBI in PMLA case</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>https://www.yahoo.com/finance/news/cdk-global-files-lawsuit-against-191842547.html</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>CDK Global files lawsuit against Tekion over alleged cyber hacking campaign</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/hareholder-alert-the-ma-class-action-firm-continues-to-investigate-the-merger--evgr-qtrx-rkda-ebtc-302377462.html</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>$HAREHOLDER ALERT: The M&amp;A Class Action Firm Continues To Investigate The Merger - EVGR, QTRX, RKDA, EBTC</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>https://www.wealthmanagement.com/wealth-management-industry-trends/investment-fraud-suit-brought-by-brokers-blocked-by-the-supremes</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Investment Fraud Suit Brought By Brokers Blocked By The Supremes</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>https://www.wealthmanagement.com/regulation-compliance/investment-advisor-gets-more-than-five-years-in-prison-for-securities-fraud</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Investment Advisor Gets More Than Five Years in Prison for Securities Fraud</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>https://www.deccanchronicle.com/nation/crime/bank-general-manager-arrested-for-siphoning-rs-122-crore-1861499</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Bank General Manager Arrested for Siphoning Rs 122 Crore</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>https://www.chilkatvalleynews.com/2025/02/15/new-lawsuit-seeks-to-limit-alaska-native-tribes-authority-stop-eklutna-gambling-hall/</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>New lawsuit seeks to limit Alaska Native tribes’ authority, stop Eklutna gambling hall</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>https://www.morningstar.com/news/pr-newswire/20250215dc19920/tgt-investors-have-opportunity-to-lead-target-corporation-securities-fraud-lawsuit</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>TGT Investors Have Opportunity to Lead Target Corporation Securities Fraud Lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>https://www.lancs.live/news/lancashire-news/law-firm-ordered-pay-30k-30939354</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Law firm ordered to pay £30k after falling foul of money laundering risk rules</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>https://www.morningstar.com/news/pr-newswire/20250213ny18143/investors-in-modivcare-inc-should-contact-the-gross-law-firm-before-march-31-2025-to-discuss-your-rights-modv</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Investors in ModivCare Inc. Should Contact The Gross Law Firm Before March 31, 2025 to Discuss Your Rights - MODV</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>https://www.globenewswire.com/news-release/2025/02/12/3025319/0/en/The-Gross-Law-Firm-Reminds-Shareholders-of-a-Lead-Plaintiff-Deadline-of-March-18-2025-in-Block-Inc-Lawsuit-XYZ.html</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>The Gross Law Firm Reminds Shareholders of a Lead Plaintiff Deadline of March 18, 2025 in Block, Inc. Lawsuit – XYZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>https://www.recoilweb.com/ke-arms-brownells-and-others-sued-by-anti-ar-15-investor-175976.html</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>KE Arms, Brownells, And Others Sued By Anti-AR-15 Investor [UPDATE: VICTORY]</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>https://www.kpax.com/news/montana-news/hamilton-lawmaker-files-suit-against-big-tobacco-for-flouting-law</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Hamilton lawmaker files suit against ‘Big Tobacco’ for flouting law</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/kessler-topaz-meltzer--check-llp-encourages-grocery-outlet-holding-corp-investors-with-losses-to-contact-the-firm-302375261.html</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Kessler Topaz Meltzer &amp; Check, LLP Encourages Grocery Outlet Holding Corp. Investors with Losses to Contact the Firm</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/proposed-smithsonian-italian-american-museum-rallies-national-support-as-us-house-weighs-legislation-302377565.html</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Proposed Smithsonian Italian American Museum Rallies National Support as US House Weighs Legislation</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>https://www.abc27.com/news/us-world/business/ppl-non-financial-customer-data-involved-in-2023-breach-company-says/</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>PPL non-financial customer data involved in 2023 breach, company says</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>https://www.dailymail.co.uk/news/article-14400959/Probe-teacher-accused-misconduct-lasted-EIGHT-YEARS.html</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Probe into a teacher accused of misconduct has lasted more than EIGHT YEARS</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>https://world.thaipbs.or.th/detail/56538</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>44 former Move Forward MPs face ethical misconduct charges</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>https://www.newsbreak.com/morristown-minute-1590138/3812566470597-suspended-police-chief-convicted-of-misconduct-and-sexual-assault</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Suspended Police Chief Convicted of Misconduct and Sexual Assault</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>https://www.newsbreak.com/the-center-square-509740/3814418961378-chicago-pays-millions-in-2024-to-settle-police-misconduct-suits</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Chicago pays millions in 2024 to settle police misconduct suits</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>https://www.footboom1.com/en/news/football/2377617-gerard-pique-to-face-court-over-financial-misconduct-in-spanish-super-cup-scandal</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Gerard Piqué to Face Court Over Financial Misconduct in Spanish Super Cup Scandal</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>https://www.buzzfeed.com/larryfitzmaurice/jay-z-responds-sexual-assault-lawsuit-dismissal</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Jay-Z Issued A Fiery Statement In Response To The Sexual Assault Lawsuit Against Him Being Dropped</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>https://www.logandaily.com/news/property-owner-prevails-in-lawsuit-over-big-land-sale-that-fell-through/article_f6fd28f6-ebbe-11ef-85ac-7b3b07cca1fe.html</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Property owner prevails in lawsuit over big land sale that fell through</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>https://www.cbsnews.com/newyork/news/doge-lawsuit-new-york-elon-musk-treasury/</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>At DOGE lawsuit hearing in New York, state attorneys general allege largest data breach in U.S. history</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>https://www.dailymail.co.uk/news/article-14400929/pam-bondi-backlash-eric-adams-scandal.html</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Pam Bondi faces conservative backlash over Eric Adams 'scandal'</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>https://www.taipeitimes.com/News/world/archives/2025/02/16/2003831980</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Mexico threatens US gunmakers with legal action</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>https://kyma.com/news/crime/2025/02/15/woman-drops-lawsuit-against-jay-z-and-diddy/</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Woman drops lawsuit against Jay-Z and Diddy</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>https://www.newindianexpress.com/states/andhra-pradesh/2025/Feb/13/ap-hc-adjourns-pil-seeking-cbi-ed-probe-against-chandrababu-naidu-ministers</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>AP HC adjourns PIL seeking CBI, ED probe against Chandrababu Naidu, ministers</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>https://www.businesswire.com/news/home/20250215155211/en/MRK-Investors-Have-Opportunity-to-Lead-Merck-Co.-Inc.-Securities-Fraud-Lawsuit-with-the-Schall-Law-Firm</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>MRK Investors Have Opportunity to Lead Merck &amp; Co., Inc. Securities Fraud Lawsuit with the Schall Law Firm</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>https://jacobin.com/2025/02/dating-apps-match-group-lawsuit/</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Dating App Giant Match Group Is Being Sued for Conning Users</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/rig-deadline-rig-investors-have-opportunity-to-lead-transocean-ltd-securities-fraud-lawsuit-302377144.html</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>RIG Deadline: RIG Investors Have Opportunity to Lead Transocean Ltd. Securities Fraud Lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>https://muslimmirror.com/jamia-displays-protesting-students-personal-info-removes-after-backlash/</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Jamia displays protesting students’ personal info, removes after backlash</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>https://www.cbsnews.com/chicago/video/man-accused-of-killing-united-healthcare-ceo-issues-message-to-supporters/</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Man accused of killing United Healthcare CEO issues message to supporters</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>https://jang.com.pk/en/31765-kanye-west-breaks-silence-as-250k-sex-tape-scandal-resurfaces-news</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Kanye West breaks silence as $250K sex tape scandal resurfaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>https://markets.financialcontent.com/stocks/article/thenewswire-2025-2-13-nxt-investor-alert-a-securities-fraud-class-action-lawsuit-has-been-filed-against-nextracker-inc-nxt</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>NXT Investor Alert: A Securities Fraud Class Action Lawsuit Has Been Filed Against Nextracker Inc. (NXT)</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>https://markets.financialcontent.com/stocks/article/thenewswire-2025-2-12-mu-investor-alert-a-securities-fraud-class-action-lawsuit-has-been-filed-against-micron-technology-inc-mu</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>MU Investor Alert: A Securities Fraud Class Action Lawsuit Has Been Filed Against Micron Technology, Inc. (MU)</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>https://www.hindustantimes.com/cities/lucknow-news/rs-50-lakh-fund-misuse-allegations-bjp-issues-show-cause-notice-to-u-p-s-fatehpur-district-president-101739638816423.html</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>₹50 lakh fund misuse allegations: BJP issues show-cause notice to U.P’s Fatehpur district president</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>https://www.thedailybeast.com/obsessed/russell-brand-shutters-charity-amid-sexual-assault-allegations/</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Russell Brand Shutters Charity Amid Sexual Assault Allegations</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>https://www.indiatodaygaming.com/news/story/bgmi-caster-mazy-under-fire-allegations-of-bullying-and-mental-harassment-shake-the-community-1-7304</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>BGMI Caster Mazy Under Fire: Allegations of Bullying and Mental Harassment Shake the Community</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>https://www.yahoo.com/news/longmont-pursue-legal-action-against-153800633.html</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Longmont to pursue legal action against contractor for construction defect issues</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>https://www.ndtv.com/india-news/mumbai-court-orders-police-probe-into-complaint-against-ekta-kapoor-7719019</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Court Orders Police To Probe Complaint Against Ekta Kapoor</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>https://ny1.com/nyc/all-boroughs/CTV/2025/02/15/trial-attorney-on-motion-to-dismiss-mayor-adams-case</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Trial attorney on motion to dismiss Mayor Adams case</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>https://www.thetravel.com/craters-of-the-moon-failed-as-idaho-national-park/</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Idaho's "Moon" Failed To Become The State's First &amp; Only National Park</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>https://www.sportskeeda.com/college-football/news-alabama-analyst-breaks-cole-adams-failed-start-year-predicting-a-positive-2025</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Alabama analyst breaks down why Cole Adams failed to start this year while predicting a positive 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>https://www.globenewswire.com/news-release/2025/02/14/3026810/32716/en/Block-Inc-XYZ-Faces-Securities-Class-Action-Regulators-Levy-Cash-App-Fines-Following-Investigations-Going-Back-to-Hindenburg-Report-Hagens-Berman.html</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Block, Inc. (XYZ) Faces Securities Class Action, Regulators</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>https://www.indexjournal.com/news/city-of-abbeville-files-lawsuit-against-calhoun-falls-over-water-contract/article_de093c5e-ebaf-11ef-8b82-b391f5718c1d.html</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>City of Abbeville files lawsuit against Calhoun Falls over water contract</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>https://www.commondreams.org/news/jd-vance-alternative-for-germany</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Vance Faces Backlash Over Embrace of Germany's Far-Right Just Ahead of Election</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>http://www.msn.com/en-us/money/other/intel-s-ai-chief-leaves-to-run-nokia-after-a-year-on-the-job/ar-AA1yJ6xu?ocid=finance-verthp-feeds&amp;apiversion=v2&amp;noservercache=1&amp;domshim=1&amp;renderwebcomponents=1&amp;wcseo=1&amp;batchservertelemetry=1&amp;noservertelemetry=1</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Nokia Picks Justin Hotard for CEO as Pekka Lundmark Exits</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>https://www.abc27.com/pennsylvania-politics/attorney-general-talks-federal-funding-lawsuit/</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Attorney General talks federal funding lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>https://www.investing.com/news/stock-market-news/uber-accuses-doordash-of-anticompetitive-practices-in-lawsuit-3871824</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Uber accuses DoorDash of anticompetitive practices in lawsuit By Reuters</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>https://www.morningstar.com/news/pr-newswire/20250215dc20126/nem-investors-have-opportunity-to-lead-newmont-corporation-securities-fraud-lawsuit</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>NEM Investors Have Opportunity to Lead Newmont Corporation Securities Fraud Lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/regn-investors-have-opportunity-to-lead-regeneron-pharmaceuticals-inc-securities-fraud-lawsuit-302377220.html</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>REGN Investors Have Opportunity to Lead Regeneron Pharmaceuticals, Inc. Securities Fraud Lawsuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>https://sapulpatimes.com/lone-star-superintendent-alerts-parents-and-employees-of-embezzlement/</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Lone Star superintendent alerts parents and employees of embezzlement</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>https://www.ndtv.com/india-news/mumbai-court-orders-police-probe-into-complaint-against-ekta-kapoor-7719019</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Court Orders Police Probe Into Complaint Against Ekta Kapoor</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/ktg-accelerates-leap-to-global-top-tier-by-reinforcing-global-operations-centered-core-competitiveness-302378502.html</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>KT&amp;G Accelerates Leap to 'Global Top-tier' by Reinforcing Global Operations-centered Core Competitiveness</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>https://milwaukeenns.org/2025/02/17/opinion-mps-failed-to-keep-our-kids-safe-and-we-should-all-be-concerned/</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Opinion: MPS failed to keep our kids safe. And we should all be concerned.</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>https://www.kktv.com/2025/02/18/mother-club-q-shooter-files-lawsuit-against-colorado-springs-police-officers/</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Mother of Club Q shooter files lawsuit against Colorado Springs Police Officers</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>https://krdo.com/news/2025/02/17/mother-of-club-q-shooter-files-civil-rights-lawsuit-against-cspd/</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Mother of Club Q shooter files civil rights lawsuit against CSPD</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>https://www.wcnc.com/video/news/local/3-year-old-allegedly-assaulted-at-daycare/275-1b4b8fff-d656-4386-88cb-14cd1cd5a06d</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Child safety concerns arise as daycare faces allegations of sex assault</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>https://www.victoriaadvocate.com/innovative-industrial-properties-inc-class-action-levi-korsinsky-reminds-innovative-industrial-properties-investors-of-the/article_2bbe5045-335e-53fa-b80b-bfc1ac8dec28.html</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Innovative Industrial Properties, Inc. Class Action: Levi &amp; Korsinsky Reminds Innovative Industrial Properties Investors of the Pending Class Action Lawsuit with a Lead Plaintiff Deadline of March 18, 2025 - IIPR</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>https://paultan.org/2025/02/18/puspakom-insists-its-compliant-with-jpj-inspection-regs-after-accused-of-failing-lorries-unreasonably/</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Puspakom insists it’s compliant with JPJ inspection regs after accused of failing lorries unreasonably</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>https://www.newsbreak.com/shefinds-518722/3815631157368-justin-bieber-reportedly-under-constant-watch-amid-alleged-substance-abuse-as-blind-item-claims-his-mother-wants-to-milk-as-much-money-from-him</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Justin Bieber Reportedly Under Constant Watch Amid Alleged Substance Abuse As Blind Item Claims His Mother Wants To 'Milk as Much Money' From Him</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>https://biztoc.com/x/b5f481d8757714fd?ref=ff</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Food Head at FDA Resigns, Citing Numerous Job Cuts in Division</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>http://guardian.pressreader.com/epaper/viewer.aspx?issue=15452025021800000000001001&amp;page=38&amp;article=2936c186-0ba0-47a4-ba1a-f4b4a6d094a1&amp;key=tEOuP0BOP8U6JyJsgZsHqQ%3d%3d&amp;feed=rss</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>18/02/2025: Sport: United malaise comes from the top and Amorim faces a battle to fix it</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>http://guardian.pressreader.com/epaper/viewer.aspx?issue=15452025021800000000001001&amp;page=39&amp;article=6240c620-dfd0-4bc2-a97e-a1852152448c&amp;key=un0P%2fYWaa7Muu2T4oJ5V3Q%3d%3d&amp;feed=rss</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>18/02/2025: Sport: FA investigating alleged racist abuse of Mejbri</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>https://www.examiner.com.au/story/8895459/west-tamar-man-charged-with-fraud-as-police-seize-four-vehicles/?src=rss</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>West Tamar man charged with fraud after police seize four vehicles</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>https://www.yahoo.com/news/fall-river-woman-admits-embezzling-191924552.html</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Fall River woman admits to embezzling $87K in Social Security benefits</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/lg-display-targets-gaming-market-with-oled-monitor-panel-featuring-worlds-best-picture-quality-302377954.html</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>LG Display Targets Gaming Market with OLED Monitor Panel featuring World's Best Picture Quality</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>https://www.globenewswire.com/news-release/2025/02/17/3027397/0/en/Regeneron-Pharmaceuticals-REGN-Faces-Securities-Class-Action-After-Losing-9-Billion-Value-Following-Q3-2024-Earnings-Report-Hagens-Berman.html</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Regeneron Pharmaceuticals (REGN) Faces Securities Class</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>https://blavity.com/stephen-twitch-boss-family-seeks-legal-counsel-allison-holker-memoir-release</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Stephen 'tWitch' Boss' Family Seeks Legal Counsel Amid Wife Allison Holker's Controversial Memoir Release</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>https://www.independent.ie/irish-news/cost-claims-by-builders-of-new-national-childrens-hospital-rise-another-100m-amid-fears-final-bill-could-still-increase/a1671673083.html</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Cost claims by builders of new National Children’s Hospital rise another €100m amid fears final bill could still increase</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>https://www.kuam.com/story/52398579/drunk-driver-charged-in-resisting-arrest</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Drunk driver charged in resisting arrest</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>https://www.hawaiinewsnow.com/2025/02/18/body-cam-video-lawsuit-shows-one-most-dangerous-police-officers/</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Body cam video in lawsuit shows ‘one of the most dangerous police officers’</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>https://www.local10.com/news/local/2025/02/18/fontainebleau-in-miami-beach-faces-lawsuit-following-2021-sexual-assault-case/</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Fontainebleau in Miami Beach faces lawsuit following 2021 sexual assault case</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>https://www.wistv.com/video/2025/02/17/lawsuit-former-camden-military-academy-dean-engaged-predatory-sexual-conduct-with-student/</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Lawsuit: Former Camden Military Academy dean engaged in ‘predatory’ sexual conduct with student</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>https://louisianaradionetwork.com/2025/02/17/lawsuit-aims-to-stop-special-election-on-constitution-changes-amid-new-tax-law/</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Lawsuit aims to stop special election on constitution changes amid new tax law</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>https://medium.com/@sdespin/the-great-social-security-heist-how-politicians-robbed-you-blind-and-blamed-everyone-but-9e8178da13e3?source=rss------politics-5</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>The Great Social Security Heist: How Politicians Robbed You Blind and Blamed Everyone but…</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>http://www.msn.com/en-gb/money/other/it-almost-destroyed-my-life-says-ni-man-defrauded-of-more-than-200000-in-romance-scam/ar-AA1yTCor?apiversion=v2&amp;noservercache=1&amp;domshim=1&amp;renderwebcomponents=1&amp;wcseo=1&amp;batchservertelemetry=1&amp;noservertelemetry=1</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>"It almost destroyed my life" says NI man defrauded of more than £200,000 in romance scam</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>https://www.koat.com/article/nba-new-mexico-university-hazing/63821877</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>'Bright future in NBA': Attorney describes sexual assault allegations as 'horseplay' in NMSU case</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>https://www.koreatimes.co.kr/www/art/2025/02/398_392447.html</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Actor Park Hee-soon denies tax evasion allegations</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>https://www.tokenpost.com/news/people/14068</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Libra Memecoin Founder Defends Project Amid Insider Trading Allegations</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>https://www.yorkshirepost.co.uk/news/crime/former-yorkshire-police-officer-jailed-after-sending-inappropriate-messages-to-crime-victim-4995621</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Former Yorkshire police officer jailed after sending inappropriate messages to crime victim</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>https://www.farmweekly.com.au/story/8894467/wa-farmer-found-guilty-under-aboriginal-heritage-act-1972/?src=rss</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Aboriginal heritage laws create chaos as first WA farmer fined for breach.</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>https://dailytrust.com/police-arrest-2-suspected-robbers-in-benue/</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Police arrest 2 suspected robbers in Benue</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>https://www.stuff.co.nz/nz-news/360585102/man-accused-violent-attack-needs-mental-health-assessed</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Man accused of violent attack needs mental health assessed</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>https://thewest.com.au/news/crime/rivervale-man-52-arrested-after-allegedly-pointing-laser-at-commercial-planes-and-police-helicopter-c-17761327</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Rivervale man, 52, arrested after allegedly pointing laser at commercial planes and police helicopter</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>https://time.com/7252981/nyc-deputy-mayors-resign-federal-involvement-adams-case/</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Four NYC Deputy Mayors Resign Over Federal Involvement in Adams Case</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>https://www.indiatoday.in/india/story/akali-dal-crisis-shiromani-gurdwara-parbandhak-committee-chief-harjinder-singh-dhami-resigns-moral-grounds-2681542-2025-02-18?utm_source=rss</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Akali Dal crisis deepens, Sikh body chief Harjinder Dhami resigns on moral grounds</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>https://edition.channel5belize.com/san-pedro-employee-charged-with-theft-of-over-500000/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=san-pedro-employee-charged-with-theft-of-over-500000</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>San Pedro Employee Charged with Theft of over $500,000</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>https://www.justice.gov/usao-ndny/pr/carla-freedman-concludes-her-service-united-states-attorney</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Carla Freedman Concludes Her Service as United States Attorney</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>https://www.globallegalpost.com/news/linklaters-hires-cma-litigation-chief-in-london-1462267709</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Linklaters hires CMA litigation chief in London</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>https://www.smh.com.au/national/western-australia/man-blinds-pilots-landing-at-perth-airport-with-laser-then-turns-it-on-police-chopper-police-allege-20250218-p5ld2p.html?ref=rss&amp;utm_medium=rss&amp;utm_source=rss_feed</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Man blinds pilots landing at Perth Airport with laser, then turns it on police chopper: police allege</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>https://www.totalprosports.com/general/womans-mugshot-breaks-the-internet-after-shes-arrested-for-filling-her-ex-boyfriends-gas-tank-with-already-sucked-skittles-coke-zero/</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Woman’s Mugshot Breaks The Internet After She’s Arrested For Filling Her Ex-Boyfriend’s Gas Tank With Already Sucked Skittles &amp; Coke Zero</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>https://biztoc.com/x/f6fb88199b688b0a?ref=ff</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Alleged Leader of 'Zizians' Group Arrested, Linked to Multiple US Killings</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>https://biztoc.com/x/51b3e4cd14961e3a?ref=ff</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Mizuho Employee Suspected of Theft in Latest Safety Box Case</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>https://www.theyeshivaworld.com/news/general/2365876/boro-park-nypd-and-shomrim-nab-mail-theft-suspects-in-early-morning-arrest.html</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>BORO PARK: NYPD and Shomrim Nab Mail Theft Suspects in Early Morning Arrest</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>https://www.credit.com/blog/questions-to-ask-debt-settlement-company/</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Questions to Ask a Debt Settlement Company</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>https://kdvr.com/news/local/deputies-chase-arrest-highly-intoxicated-man-on-i-70-during-holiday-weekend-chaos/</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Deputies chase, arrest 'highly intoxicated' man on I-70 during 'holiday weekend chaos'</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>https://www.b2bnn.com/2025/02/litigation-in-corporate-law-protecting-your-business-from-legal-disputes/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=litigation-in-corporate-law-protecting-your-business-from-legal-disputes</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Litigation in Corporate Law: Protecting Your Business from Legal Disputes</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>https://www.b2bnn.com/2025/02/how-to-prevent-theft-in-the-workplace/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=how-to-prevent-theft-in-the-workplace</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>How to Prevent Theft in the Workplace</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>https://www.abc.net.au/news/2025-02-18/katherine-local-court-judge-remand-delays-concern/104947768</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>NT judge says 'tidal wave' of arrests behind 'concerning' custody waits</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>https://www.resetera.com/threads/i-just-played-killzone-2-at-60fps-and-i-feel-like-i-should-be-arrested.1111794/</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>I just played Killzone 2 at 60FPS and I feel like I should be arrested.</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>https://www.koin.com/news/oregon/train-crashes-into-truck-in-southern-oregon-2-arrested/</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Train crashes into truck in southern Oregon; 2 arrested</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>https://www.wfla.com/news/pinellas-county/pinellas-park-tile-shop-owner-arrested-again-in-scheme-to-defraud-case/</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Pinellas Park tile shop owner arrested again in scheme to defraud case</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>https://www.globenewswire.com/news-release/2025/02/18/3027460/0/en/Kessler-Topaz-Meltzer-Check-LLP-Class-Action-Announcement-for-Neumora-Therapeutics-Inc-Investors-A-Securities-Fraud-Class-Action-Lawsuit-Was-Filed-Against-Neumora-Therapeutics-Inc.html</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Kessler Topaz Meltzer &amp; Check, LLP - Class Action Announcement for Neumora Therapeutics, Inc. Investors: A Securities Fraud Class Action Lawsuit Was Filed Against Neumora Therapeutics, Inc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>https://www.cleveland.com/community/2025/02/petty-theft-at-hobby-lobby-ends-with-arrest-of-three-women.html</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Petty theft at Hobby Lobby ends with arrest of three women</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>https://kdvr.com/news/local/northglenn-police-searching-for-man-accused-of-shoplifting-injuring-officer/</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Northglenn police searching for man accused of shoplifting, injuring officer</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>https://www.zerohedge.com/economics/missouri-truck-company-owner-gets-9-years-ppp-fraud-other-felonies</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Missouri Truck Company Owner Gets 9 Years For PPP Fraud, Other Felonies</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>https://www.nst.com.my/news/crime-courts/2025/02/1176488/man-fined%C2%A0vehicle-seized-repeatedly-colliding-another-car</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Man fined, vehicle seized for repeatedly colliding with another car</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>https://www.disneyfanatic.com/toy-story-land-woodys-lunch-box-addition-jc1/</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Disney Forever Changes Toy Story Land, Corrects Wrongdoing</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>https://www.anarchistfederation.net/person-in-crisis-dies-following-arrest-by-quebec-city-police-february-14-17-2025/</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Person in Crisis Dies Following Arrest by Quebec City Police (February 14-17, 2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>http://www.memeorandum.com/250217/p97#a250217p97</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>At least 3 NYC deputy mayors express intent to resign from Adams administration: Sources (Melissa Russo/NBC New York)</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>https://www.resetera.com/threads/ravens-kickers-justin-tucker-faces-allegations-of-sexual-misconduct-from-16-massage-therapist.1111776/</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Ravens kickers, Justin Tucker faces allegations of sexual misconduct from 16 massage therapist.</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>https://www.cleveland.com/community/2025/02/paninis-employee-to-be-charged-for-involvement-in-theft-and-cashing-of-7000-check-highland-heights-police-blotter.html</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Panini’s employee to be charged for involvement in theft and cashing of $7,000 check: Highland Heights Police Blotter</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>https://www.mydailyrecord.com/news/national/new-york-city-council-calls-for-under-fire-mayors-resignation/article_4b4d4ce8-b60a-509d-90bb-97bbf9674697.html</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>New York city council calls for under-fire mayor's resignation</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>https://biztoc.com/x/c89b56669234ab97?ref=ff</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Pervasive Police Corruption in Albuquerque Explains Why a Teetotaler Was Arrested for DWI</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>https://biztoc.com/x/4a519c009689f0c5?ref=ff</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Honda allegedly to resume merger talks if Nissan's Uchida leaves</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>https://thewest.com.au/news/boy-10-in-hospital-with-serious-injuries-after-north-liverpool-rd-crash-c-17760803</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Boy, 10, in hospital with critical injuries after North Liverpool Rd crash</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>https://www.democraticunderground.com/100220041439</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>the democrats should demand all contracts with a musk company be cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>https://www.dailybulletin.com/2025/02/17/eviction-protection-for-those-affected-by-wildfires-up-for-vote-tuesday/</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Eviction protection for those affected by wildfires up for LA County Board of Supervisors vote</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>http://rssfeeds.wusa9.com/~/913213268/0/wusa-news~VA-high-school-athletic-director-arrested-while-visiting-family-in-Pennsylvania-accused-of-sending-sexually-explicit-photos-to-underage-student</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>VA high school athletic director arrested while visiting family in Pennsylvania, accused of sending sexually explicit photos to underage student</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>https://www.newsmax.com/newsfront/nyc-council-mayor-adams-resignation/2025/02/17/id/1199429</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>New York City Council Calls for Mayor Adams' Resignation</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>https://www.scoop.co.nz/stories/AK2502/S00436/road-workers-aid-in-drunk-driver-arrest-on-sh-29.htm</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Road Workers Aid In Drunk Driver Arrest On SH 29</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>https://www.dailyexcelsior.com/three-held-for-theft-stolen-property-recovered/</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Three held for theft, stolen property recovered</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>https://www.wallstreet-online.de/nachricht/19011320-alaska-energy-metals-announces-resignation-of-director</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Alaska Energy Metals Announces Resignation Of Director</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>https://www.globenewswire.com/news-release/2025/02/18/3027447/673/en/ROSEN-A-LEADING-INVESTOR-RIGHTS-LAW-FIRM-Encourages-Alarum-Technologies-Ltd-Investors-to-Secure-Counsel-Before-Important-Deadline-in-Securities-Class-Action-ALAR.html</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>ROSEN, A LEADING INVESTOR RIGHTS LAW FIRM, Encourages Alarum Technologies Ltd. Investors to Secure Counsel Before Important Deadline in Securities Class Action – ALAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>https://7news.com.au/news/man-arrested-after-woman-dies-in-hospital-with-serious-injuries-c-17760100</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Man arrested after woman dies in hospital with ‘serious injuries’</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>https://www.villages-news.com/2025/02/17/suspect-arrested-in-theft-at-construction-site-in-the-villages/</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Suspect arrested in theft at construction site in The Villages</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>https://thisisreno.com/2025/02/washoe-county-homelessness-reduction-innaccurate/</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Fact-Check: Did Washoe County mislead the legislature on homeless numbers? Yes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>https://biztoc.com/x/517eeb2650f32d24?ref=ff</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Does car insurance cover theft?</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>